<commit_message>
fix(All over the place): Fixes for the new export
</commit_message>
<xml_diff>
--- a/emx/vkgl-model.xlsx
+++ b/emx/vkgl-model.xlsx
@@ -11,7 +11,7 @@
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="packages" sheetId="3" r:id="rId3"/>
     <sheet name="vkgl_classification" sheetId="7" r:id="rId4"/>
-    <sheet name="vkgl_public_classificiation" sheetId="8" r:id="rId5"/>
+    <sheet name="vkgl_public_classification" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="247">
   <si>
     <t>entity</t>
   </si>
@@ -698,6 +698,72 @@
   </si>
   <si>
     <t>LP</t>
+  </si>
+  <si>
+    <t>hgvs_normalized_vkgl</t>
+  </si>
+  <si>
+    <t>ref_orig</t>
+  </si>
+  <si>
+    <t>alt_orig</t>
+  </si>
+  <si>
+    <t>raw_amc_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_alissa_model_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_lumc_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_radboud_v2</t>
+  </si>
+  <si>
+    <t>raw_erasmus_v2</t>
+  </si>
+  <si>
+    <t>raw_umcg_v2</t>
+  </si>
+  <si>
+    <t>raw_umcu_v2</t>
+  </si>
+  <si>
+    <t>raw_vumc_v2</t>
+  </si>
+  <si>
+    <t>raw_nki_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_umcu_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_umcg_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_vumc_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_erasmus_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_amc_v2</t>
+  </si>
+  <si>
+    <t>vkgl_raw_nki_v2</t>
+  </si>
+  <si>
+    <t>raw_alissa_model_v2</t>
+  </si>
+  <si>
+    <t>Raw alissa model v2</t>
+  </si>
+  <si>
+    <t>hgvs_normalized</t>
+  </si>
+  <si>
+    <t>chromosome_orig</t>
   </si>
 </sst>
 </file>
@@ -741,7 +807,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -784,6 +850,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -794,7 +890,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -876,8 +972,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -887,8 +1027,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -929,6 +1074,28 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -969,6 +1136,28 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1298,11 +1487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK160"/>
+  <dimension ref="A1:AK225"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U159" sqref="U159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6763,9 +6952,1349 @@
         <v>1</v>
       </c>
     </row>
+    <row r="161" spans="1:19" s="9" customFormat="1">
+      <c r="A161" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G161" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="S161" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19" s="9" customFormat="1">
+      <c r="A162" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="163" spans="1:19" s="9" customFormat="1">
+      <c r="A163" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="164" spans="1:19" s="9" customFormat="1">
+      <c r="A164" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19" s="9" customFormat="1">
+      <c r="A165" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B165" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D165" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19" s="9" customFormat="1">
+      <c r="A166" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D166" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19" s="9" customFormat="1">
+      <c r="A167" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="168" spans="1:19" s="9" customFormat="1">
+      <c r="A168" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="169" spans="1:19" s="9" customFormat="1">
+      <c r="A169" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B169" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19" s="9" customFormat="1">
+      <c r="A170" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19" s="9" customFormat="1">
+      <c r="A171" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19" s="9" customFormat="1">
+      <c r="A172" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B172" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="173" spans="1:19" s="9" customFormat="1">
+      <c r="A173" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B173" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="174" spans="1:19" s="9" customFormat="1">
+      <c r="A174" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B174" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="175" spans="1:19" s="9" customFormat="1">
+      <c r="A175" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B175" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19" s="9" customFormat="1">
+      <c r="A176" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B176" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="177" spans="1:37" s="9" customFormat="1">
+      <c r="A177" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B177" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="178" spans="1:37" s="9" customFormat="1">
+      <c r="A178" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="179" spans="1:37" s="9" customFormat="1">
+      <c r="A179" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B179" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" spans="1:37" s="9" customFormat="1">
+      <c r="A180" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B180" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="1:37" s="9" customFormat="1">
+      <c r="A181" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B181" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="182" spans="1:37" s="9" customFormat="1">
+      <c r="A182" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B182" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="183" spans="1:37" s="9" customFormat="1">
+      <c r="A183" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B183" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="184" spans="1:37" s="9" customFormat="1">
+      <c r="A184" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B184" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="185" spans="1:37" s="11" customFormat="1">
+      <c r="A185" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C185" s="10"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="10"/>
+      <c r="F185" s="10"/>
+      <c r="G185" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H185" s="10"/>
+      <c r="I185" s="10"/>
+      <c r="J185" s="10"/>
+      <c r="K185" s="10"/>
+      <c r="L185" s="10"/>
+      <c r="M185" s="10"/>
+      <c r="N185" s="10"/>
+      <c r="O185" s="10"/>
+      <c r="P185" s="10"/>
+      <c r="Q185" s="10"/>
+      <c r="R185" s="10"/>
+      <c r="S185" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T185" s="10"/>
+      <c r="U185" s="10"/>
+      <c r="V185" s="10"/>
+      <c r="W185" s="10"/>
+      <c r="X185" s="10"/>
+      <c r="Y185" s="10"/>
+      <c r="Z185" s="10"/>
+      <c r="AA185" s="10"/>
+      <c r="AB185" s="10"/>
+      <c r="AC185" s="10"/>
+      <c r="AD185" s="10"/>
+      <c r="AE185" s="10"/>
+      <c r="AF185" s="10"/>
+      <c r="AG185" s="10"/>
+      <c r="AH185" s="10"/>
+      <c r="AI185" s="10"/>
+      <c r="AJ185" s="10"/>
+      <c r="AK185" s="10"/>
+    </row>
+    <row r="186" spans="1:37" s="11" customFormat="1">
+      <c r="A186" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C186" s="10"/>
+      <c r="D186" s="10"/>
+      <c r="E186" s="10"/>
+      <c r="F186" s="10"/>
+      <c r="G186" s="10"/>
+      <c r="H186" s="10"/>
+      <c r="I186" s="10"/>
+      <c r="J186" s="10"/>
+      <c r="K186" s="10"/>
+      <c r="L186" s="10"/>
+      <c r="M186" s="10"/>
+      <c r="N186" s="10"/>
+      <c r="O186" s="10"/>
+      <c r="P186" s="10"/>
+      <c r="Q186" s="10"/>
+      <c r="R186" s="10"/>
+      <c r="S186" s="10"/>
+      <c r="T186" s="10"/>
+      <c r="U186" s="10"/>
+      <c r="V186" s="10"/>
+      <c r="W186" s="10"/>
+      <c r="X186" s="10"/>
+      <c r="Y186" s="10"/>
+      <c r="Z186" s="10"/>
+      <c r="AA186" s="10"/>
+      <c r="AB186" s="10"/>
+      <c r="AC186" s="10"/>
+      <c r="AD186" s="10"/>
+      <c r="AE186" s="10"/>
+      <c r="AF186" s="10"/>
+      <c r="AG186" s="10"/>
+      <c r="AH186" s="10"/>
+      <c r="AI186" s="10"/>
+      <c r="AJ186" s="10"/>
+      <c r="AK186" s="10"/>
+    </row>
+    <row r="187" spans="1:37" s="11" customFormat="1">
+      <c r="A187" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B187" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C187" s="10"/>
+      <c r="D187" s="10"/>
+      <c r="E187" s="10"/>
+      <c r="F187" s="10"/>
+      <c r="G187" s="10"/>
+      <c r="H187" s="10"/>
+      <c r="I187" s="10"/>
+      <c r="J187" s="10"/>
+      <c r="K187" s="10"/>
+      <c r="L187" s="10"/>
+      <c r="M187" s="10"/>
+      <c r="N187" s="10"/>
+      <c r="O187" s="10"/>
+      <c r="P187" s="10"/>
+      <c r="Q187" s="10"/>
+      <c r="R187" s="10"/>
+      <c r="S187" s="10"/>
+      <c r="T187" s="10"/>
+      <c r="U187" s="10"/>
+      <c r="V187" s="10"/>
+      <c r="W187" s="10"/>
+      <c r="X187" s="10"/>
+      <c r="Y187" s="10"/>
+      <c r="Z187" s="10"/>
+      <c r="AA187" s="10"/>
+      <c r="AB187" s="10"/>
+      <c r="AC187" s="10"/>
+      <c r="AD187" s="10"/>
+      <c r="AE187" s="10"/>
+      <c r="AF187" s="10"/>
+      <c r="AG187" s="10"/>
+      <c r="AH187" s="10"/>
+      <c r="AI187" s="10"/>
+      <c r="AJ187" s="10"/>
+      <c r="AK187" s="10"/>
+    </row>
+    <row r="188" spans="1:37" s="11" customFormat="1">
+      <c r="A188" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B188" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C188" s="10"/>
+      <c r="D188" s="10"/>
+      <c r="E188" s="10"/>
+      <c r="F188" s="10"/>
+      <c r="G188" s="10"/>
+      <c r="H188" s="10"/>
+      <c r="I188" s="10"/>
+      <c r="J188" s="10"/>
+      <c r="K188" s="10"/>
+      <c r="L188" s="10"/>
+      <c r="M188" s="10"/>
+      <c r="N188" s="10"/>
+      <c r="O188" s="10"/>
+      <c r="P188" s="10"/>
+      <c r="Q188" s="10"/>
+      <c r="R188" s="10"/>
+      <c r="S188" s="10"/>
+      <c r="T188" s="10"/>
+      <c r="U188" s="10"/>
+      <c r="V188" s="10"/>
+      <c r="W188" s="10"/>
+      <c r="X188" s="10"/>
+      <c r="Y188" s="10"/>
+      <c r="Z188" s="10"/>
+      <c r="AA188" s="10"/>
+      <c r="AB188" s="10"/>
+      <c r="AC188" s="10"/>
+      <c r="AD188" s="10"/>
+      <c r="AE188" s="10"/>
+      <c r="AF188" s="10"/>
+      <c r="AG188" s="10"/>
+      <c r="AH188" s="10"/>
+      <c r="AI188" s="10"/>
+      <c r="AJ188" s="10"/>
+      <c r="AK188" s="10"/>
+    </row>
+    <row r="189" spans="1:37" s="11" customFormat="1">
+      <c r="A189" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B189" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C189" s="10"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
+      <c r="F189" s="10"/>
+      <c r="G189" s="10"/>
+      <c r="H189" s="10"/>
+      <c r="I189" s="10"/>
+      <c r="J189" s="10"/>
+      <c r="K189" s="10"/>
+      <c r="L189" s="10"/>
+      <c r="M189" s="10"/>
+      <c r="N189" s="10"/>
+      <c r="O189" s="10"/>
+      <c r="P189" s="10"/>
+      <c r="Q189" s="10"/>
+      <c r="R189" s="10"/>
+      <c r="S189" s="10"/>
+      <c r="T189" s="10"/>
+      <c r="U189" s="10"/>
+      <c r="V189" s="10"/>
+      <c r="W189" s="10"/>
+      <c r="X189" s="10"/>
+      <c r="Y189" s="10"/>
+      <c r="Z189" s="10"/>
+      <c r="AA189" s="10"/>
+      <c r="AB189" s="10"/>
+      <c r="AC189" s="10"/>
+      <c r="AD189" s="10"/>
+      <c r="AE189" s="10"/>
+      <c r="AF189" s="10"/>
+      <c r="AG189" s="10"/>
+      <c r="AH189" s="10"/>
+      <c r="AI189" s="10"/>
+      <c r="AJ189" s="10"/>
+      <c r="AK189" s="10"/>
+    </row>
+    <row r="190" spans="1:37" s="11" customFormat="1">
+      <c r="A190" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C190" s="10"/>
+      <c r="D190" s="10"/>
+      <c r="E190" s="10"/>
+      <c r="F190" s="10"/>
+      <c r="G190" s="10"/>
+      <c r="H190" s="10"/>
+      <c r="I190" s="10"/>
+      <c r="J190" s="10"/>
+      <c r="K190" s="10"/>
+      <c r="L190" s="10"/>
+      <c r="M190" s="10"/>
+      <c r="N190" s="10"/>
+      <c r="O190" s="10"/>
+      <c r="P190" s="10"/>
+      <c r="Q190" s="10"/>
+      <c r="R190" s="10"/>
+      <c r="S190" s="10"/>
+      <c r="T190" s="10"/>
+      <c r="U190" s="10"/>
+      <c r="V190" s="10"/>
+      <c r="W190" s="10"/>
+      <c r="X190" s="10"/>
+      <c r="Y190" s="10"/>
+      <c r="Z190" s="10"/>
+      <c r="AA190" s="10"/>
+      <c r="AB190" s="10"/>
+      <c r="AC190" s="10"/>
+      <c r="AD190" s="10"/>
+      <c r="AE190" s="10"/>
+      <c r="AF190" s="10"/>
+      <c r="AG190" s="10"/>
+      <c r="AH190" s="10"/>
+      <c r="AI190" s="10"/>
+      <c r="AJ190" s="10"/>
+      <c r="AK190" s="10"/>
+    </row>
+    <row r="191" spans="1:37" s="11" customFormat="1">
+      <c r="A191" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B191" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C191" s="10"/>
+      <c r="D191" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E191" s="10"/>
+      <c r="F191" s="10"/>
+      <c r="G191" s="10"/>
+      <c r="H191" s="10"/>
+      <c r="I191" s="10"/>
+      <c r="J191" s="10"/>
+      <c r="K191" s="10"/>
+      <c r="L191" s="10"/>
+      <c r="M191" s="10"/>
+      <c r="N191" s="10"/>
+      <c r="O191" s="10"/>
+      <c r="P191" s="10"/>
+      <c r="Q191" s="10"/>
+      <c r="R191" s="10"/>
+      <c r="S191" s="10"/>
+      <c r="T191" s="10"/>
+      <c r="U191" s="10"/>
+      <c r="V191" s="10"/>
+      <c r="W191" s="10"/>
+      <c r="X191" s="10"/>
+      <c r="Y191" s="10"/>
+      <c r="Z191" s="10"/>
+      <c r="AA191" s="10"/>
+      <c r="AB191" s="10"/>
+      <c r="AC191" s="10"/>
+      <c r="AD191" s="10"/>
+      <c r="AE191" s="10"/>
+      <c r="AF191" s="10"/>
+      <c r="AG191" s="10"/>
+      <c r="AH191" s="10"/>
+      <c r="AI191" s="10"/>
+      <c r="AJ191" s="10"/>
+      <c r="AK191" s="10"/>
+    </row>
+    <row r="192" spans="1:37" s="11" customFormat="1">
+      <c r="A192" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B192" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C192" s="10"/>
+      <c r="D192" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E192" s="10"/>
+      <c r="F192" s="10"/>
+      <c r="G192" s="10"/>
+      <c r="H192" s="10"/>
+      <c r="I192" s="10"/>
+      <c r="J192" s="10"/>
+      <c r="K192" s="10"/>
+      <c r="L192" s="10"/>
+      <c r="M192" s="10"/>
+      <c r="N192" s="10"/>
+      <c r="O192" s="10"/>
+      <c r="P192" s="10"/>
+      <c r="Q192" s="10"/>
+      <c r="R192" s="10"/>
+      <c r="S192" s="10"/>
+      <c r="T192" s="10"/>
+      <c r="U192" s="10"/>
+      <c r="V192" s="10"/>
+      <c r="W192" s="10"/>
+      <c r="X192" s="10"/>
+      <c r="Y192" s="10"/>
+      <c r="Z192" s="10"/>
+      <c r="AA192" s="10"/>
+      <c r="AB192" s="10"/>
+      <c r="AC192" s="10"/>
+      <c r="AD192" s="10"/>
+      <c r="AE192" s="10"/>
+      <c r="AF192" s="10"/>
+      <c r="AG192" s="10"/>
+      <c r="AH192" s="10"/>
+      <c r="AI192" s="10"/>
+      <c r="AJ192" s="10"/>
+      <c r="AK192" s="10"/>
+    </row>
+    <row r="193" spans="1:37" s="11" customFormat="1">
+      <c r="A193" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B193" s="11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="194" spans="1:37" s="11" customFormat="1">
+      <c r="A194" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B194" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="195" spans="1:37" s="11" customFormat="1">
+      <c r="A195" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B195" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="196" spans="1:37" s="11" customFormat="1">
+      <c r="A196" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B196" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="197" spans="1:37" s="11" customFormat="1">
+      <c r="A197" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B197" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="198" spans="1:37" s="11" customFormat="1">
+      <c r="A198" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B198" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="199" spans="1:37" s="11" customFormat="1">
+      <c r="A199" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B199" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="200" spans="1:37" s="13" customFormat="1">
+      <c r="A200" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B200" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C200" s="12"/>
+      <c r="D200" s="12"/>
+      <c r="E200" s="12"/>
+      <c r="F200" s="12"/>
+      <c r="G200" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="H200" s="12"/>
+      <c r="I200" s="12"/>
+      <c r="J200" s="12"/>
+      <c r="K200" s="12"/>
+      <c r="L200" s="12"/>
+      <c r="M200" s="12"/>
+      <c r="N200" s="12"/>
+      <c r="O200" s="12"/>
+      <c r="P200" s="12"/>
+      <c r="Q200" s="12"/>
+      <c r="R200" s="12"/>
+      <c r="S200" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T200" s="12"/>
+      <c r="U200" s="12"/>
+      <c r="V200" s="12"/>
+      <c r="W200" s="12"/>
+      <c r="X200" s="12"/>
+      <c r="Y200" s="12"/>
+      <c r="Z200" s="12"/>
+      <c r="AA200" s="12"/>
+      <c r="AB200" s="12"/>
+      <c r="AC200" s="12"/>
+      <c r="AD200" s="12"/>
+      <c r="AE200" s="12"/>
+      <c r="AF200" s="12"/>
+      <c r="AG200" s="12"/>
+      <c r="AH200" s="12"/>
+      <c r="AI200" s="12"/>
+      <c r="AJ200" s="12"/>
+      <c r="AK200" s="12"/>
+    </row>
+    <row r="201" spans="1:37" s="13" customFormat="1">
+      <c r="A201" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B201" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C201" s="12"/>
+      <c r="D201" s="12"/>
+      <c r="E201" s="12"/>
+      <c r="F201" s="12"/>
+      <c r="G201" s="12"/>
+      <c r="H201" s="12"/>
+      <c r="I201" s="12"/>
+      <c r="J201" s="12"/>
+      <c r="K201" s="12"/>
+      <c r="L201" s="12"/>
+      <c r="M201" s="12"/>
+      <c r="N201" s="12"/>
+      <c r="O201" s="12"/>
+      <c r="P201" s="12"/>
+      <c r="Q201" s="12"/>
+      <c r="R201" s="12"/>
+      <c r="S201" s="12"/>
+      <c r="T201" s="12"/>
+      <c r="U201" s="12"/>
+      <c r="V201" s="12"/>
+      <c r="W201" s="12"/>
+      <c r="X201" s="12"/>
+      <c r="Y201" s="12"/>
+      <c r="Z201" s="12"/>
+      <c r="AA201" s="12"/>
+      <c r="AB201" s="12"/>
+      <c r="AC201" s="12"/>
+      <c r="AD201" s="12"/>
+      <c r="AE201" s="12"/>
+      <c r="AF201" s="12"/>
+      <c r="AG201" s="12"/>
+      <c r="AH201" s="12"/>
+      <c r="AI201" s="12"/>
+      <c r="AJ201" s="12"/>
+      <c r="AK201" s="12"/>
+    </row>
+    <row r="202" spans="1:37" s="13" customFormat="1">
+      <c r="A202" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B202" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C202" s="12"/>
+      <c r="D202" s="12"/>
+      <c r="E202" s="12"/>
+      <c r="F202" s="12"/>
+      <c r="G202" s="12"/>
+      <c r="H202" s="12"/>
+      <c r="I202" s="12"/>
+      <c r="J202" s="12"/>
+      <c r="K202" s="12"/>
+      <c r="L202" s="12"/>
+      <c r="M202" s="12"/>
+      <c r="N202" s="12"/>
+      <c r="O202" s="12"/>
+      <c r="P202" s="12"/>
+      <c r="Q202" s="12"/>
+      <c r="R202" s="12"/>
+      <c r="S202" s="12"/>
+      <c r="T202" s="12"/>
+      <c r="U202" s="12"/>
+      <c r="V202" s="12"/>
+      <c r="W202" s="12"/>
+      <c r="X202" s="12"/>
+      <c r="Y202" s="12"/>
+      <c r="Z202" s="12"/>
+      <c r="AA202" s="12"/>
+      <c r="AB202" s="12"/>
+      <c r="AC202" s="12"/>
+      <c r="AD202" s="12"/>
+      <c r="AE202" s="12"/>
+      <c r="AF202" s="12"/>
+      <c r="AG202" s="12"/>
+      <c r="AH202" s="12"/>
+      <c r="AI202" s="12"/>
+      <c r="AJ202" s="12"/>
+      <c r="AK202" s="12"/>
+    </row>
+    <row r="203" spans="1:37" s="13" customFormat="1">
+      <c r="A203" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B203" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C203" s="12"/>
+      <c r="D203" s="12"/>
+      <c r="E203" s="12"/>
+      <c r="F203" s="12"/>
+      <c r="G203" s="12"/>
+      <c r="H203" s="12"/>
+      <c r="I203" s="12"/>
+      <c r="J203" s="12"/>
+      <c r="K203" s="12"/>
+      <c r="L203" s="12"/>
+      <c r="M203" s="12"/>
+      <c r="N203" s="12"/>
+      <c r="O203" s="12"/>
+      <c r="P203" s="12"/>
+      <c r="Q203" s="12"/>
+      <c r="R203" s="12"/>
+      <c r="S203" s="12"/>
+      <c r="T203" s="12"/>
+      <c r="U203" s="12"/>
+      <c r="V203" s="12"/>
+      <c r="W203" s="12"/>
+      <c r="X203" s="12"/>
+      <c r="Y203" s="12"/>
+      <c r="Z203" s="12"/>
+      <c r="AA203" s="12"/>
+      <c r="AB203" s="12"/>
+      <c r="AC203" s="12"/>
+      <c r="AD203" s="12"/>
+      <c r="AE203" s="12"/>
+      <c r="AF203" s="12"/>
+      <c r="AG203" s="12"/>
+      <c r="AH203" s="12"/>
+      <c r="AI203" s="12"/>
+      <c r="AJ203" s="12"/>
+      <c r="AK203" s="12"/>
+    </row>
+    <row r="204" spans="1:37" s="13" customFormat="1">
+      <c r="A204" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B204" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C204" s="12"/>
+      <c r="D204" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E204" s="12"/>
+      <c r="F204" s="12"/>
+      <c r="G204" s="12"/>
+      <c r="H204" s="12"/>
+      <c r="I204" s="12"/>
+      <c r="J204" s="12"/>
+      <c r="K204" s="12"/>
+      <c r="L204" s="12"/>
+      <c r="M204" s="12"/>
+      <c r="N204" s="12"/>
+      <c r="O204" s="12"/>
+      <c r="P204" s="12"/>
+      <c r="Q204" s="12"/>
+      <c r="R204" s="12"/>
+      <c r="S204" s="12"/>
+      <c r="T204" s="12"/>
+      <c r="U204" s="12"/>
+      <c r="V204" s="12"/>
+      <c r="W204" s="12"/>
+      <c r="X204" s="12"/>
+      <c r="Y204" s="12"/>
+      <c r="Z204" s="12"/>
+      <c r="AA204" s="12"/>
+      <c r="AB204" s="12"/>
+      <c r="AC204" s="12"/>
+      <c r="AD204" s="12"/>
+      <c r="AE204" s="12"/>
+      <c r="AF204" s="12"/>
+      <c r="AG204" s="12"/>
+      <c r="AH204" s="12"/>
+      <c r="AI204" s="12"/>
+      <c r="AJ204" s="12"/>
+      <c r="AK204" s="12"/>
+    </row>
+    <row r="205" spans="1:37" s="13" customFormat="1">
+      <c r="A205" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B205" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C205" s="12"/>
+      <c r="D205" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E205" s="12"/>
+      <c r="F205" s="12"/>
+      <c r="G205" s="12"/>
+      <c r="H205" s="12"/>
+      <c r="I205" s="12"/>
+      <c r="J205" s="12"/>
+      <c r="K205" s="12"/>
+      <c r="L205" s="12"/>
+      <c r="M205" s="12"/>
+      <c r="N205" s="12"/>
+      <c r="O205" s="12"/>
+      <c r="P205" s="12"/>
+      <c r="Q205" s="12"/>
+      <c r="R205" s="12"/>
+      <c r="S205" s="12"/>
+      <c r="T205" s="12"/>
+      <c r="U205" s="12"/>
+      <c r="V205" s="12"/>
+      <c r="W205" s="12"/>
+      <c r="X205" s="12"/>
+      <c r="Y205" s="12"/>
+      <c r="Z205" s="12"/>
+      <c r="AA205" s="12"/>
+      <c r="AB205" s="12"/>
+      <c r="AC205" s="12"/>
+      <c r="AD205" s="12"/>
+      <c r="AE205" s="12"/>
+      <c r="AF205" s="12"/>
+      <c r="AG205" s="12"/>
+      <c r="AH205" s="12"/>
+      <c r="AI205" s="12"/>
+      <c r="AJ205" s="12"/>
+      <c r="AK205" s="12"/>
+    </row>
+    <row r="206" spans="1:37" s="13" customFormat="1">
+      <c r="A206" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B206" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C206" s="12"/>
+      <c r="D206" s="12"/>
+      <c r="E206" s="12"/>
+      <c r="F206" s="12"/>
+      <c r="G206" s="12"/>
+      <c r="H206" s="12"/>
+      <c r="I206" s="12"/>
+      <c r="J206" s="12"/>
+      <c r="K206" s="12"/>
+      <c r="L206" s="12"/>
+      <c r="M206" s="12"/>
+      <c r="N206" s="12"/>
+      <c r="O206" s="12"/>
+      <c r="P206" s="12"/>
+      <c r="Q206" s="12"/>
+      <c r="R206" s="12"/>
+      <c r="S206" s="12"/>
+      <c r="T206" s="12"/>
+      <c r="U206" s="12"/>
+      <c r="V206" s="12"/>
+      <c r="W206" s="12"/>
+      <c r="X206" s="12"/>
+      <c r="Y206" s="12"/>
+      <c r="Z206" s="12"/>
+      <c r="AA206" s="12"/>
+      <c r="AB206" s="12"/>
+      <c r="AC206" s="12"/>
+      <c r="AD206" s="12"/>
+      <c r="AE206" s="12"/>
+      <c r="AF206" s="12"/>
+      <c r="AG206" s="12"/>
+      <c r="AH206" s="12"/>
+      <c r="AI206" s="12"/>
+      <c r="AJ206" s="12"/>
+      <c r="AK206" s="12"/>
+    </row>
+    <row r="207" spans="1:37" s="13" customFormat="1">
+      <c r="A207" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B207" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C207" s="12"/>
+      <c r="D207" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E207" s="12"/>
+      <c r="F207" s="12"/>
+      <c r="G207" s="12"/>
+      <c r="H207" s="12"/>
+      <c r="I207" s="12"/>
+      <c r="J207" s="12"/>
+      <c r="K207" s="12"/>
+      <c r="L207" s="12"/>
+      <c r="M207" s="12"/>
+      <c r="N207" s="12"/>
+      <c r="O207" s="12"/>
+      <c r="P207" s="12"/>
+      <c r="Q207" s="12"/>
+      <c r="R207" s="12"/>
+      <c r="S207" s="12"/>
+      <c r="T207" s="12"/>
+      <c r="U207" s="12"/>
+      <c r="V207" s="12"/>
+      <c r="W207" s="12"/>
+      <c r="X207" s="12"/>
+      <c r="Y207" s="12"/>
+      <c r="Z207" s="12"/>
+      <c r="AA207" s="12"/>
+      <c r="AB207" s="12"/>
+      <c r="AC207" s="12"/>
+      <c r="AD207" s="12"/>
+      <c r="AE207" s="12"/>
+      <c r="AF207" s="12"/>
+      <c r="AG207" s="12"/>
+      <c r="AH207" s="12"/>
+      <c r="AI207" s="12"/>
+      <c r="AJ207" s="12"/>
+      <c r="AK207" s="12"/>
+    </row>
+    <row r="208" spans="1:37" s="13" customFormat="1">
+      <c r="A208" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B208" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C208" s="12"/>
+      <c r="D208" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E208" s="12"/>
+      <c r="F208" s="12"/>
+      <c r="G208" s="12"/>
+      <c r="H208" s="12"/>
+      <c r="I208" s="12"/>
+      <c r="J208" s="12"/>
+      <c r="K208" s="12"/>
+      <c r="L208" s="12"/>
+      <c r="M208" s="12"/>
+      <c r="N208" s="12"/>
+      <c r="O208" s="12"/>
+      <c r="P208" s="12"/>
+      <c r="Q208" s="12"/>
+      <c r="R208" s="12"/>
+      <c r="S208" s="12"/>
+      <c r="T208" s="12"/>
+      <c r="U208" s="12"/>
+      <c r="V208" s="12"/>
+      <c r="W208" s="12"/>
+      <c r="X208" s="12"/>
+      <c r="Y208" s="12"/>
+      <c r="Z208" s="12"/>
+      <c r="AA208" s="12"/>
+      <c r="AB208" s="12"/>
+      <c r="AC208" s="12"/>
+      <c r="AD208" s="12"/>
+      <c r="AE208" s="12"/>
+      <c r="AF208" s="12"/>
+      <c r="AG208" s="12"/>
+      <c r="AH208" s="12"/>
+      <c r="AI208" s="12"/>
+      <c r="AJ208" s="12"/>
+      <c r="AK208" s="12"/>
+    </row>
+    <row r="209" spans="1:37" s="13" customFormat="1">
+      <c r="A209" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B209" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C209" s="12"/>
+      <c r="D209" s="12"/>
+      <c r="E209" s="12"/>
+      <c r="F209" s="12"/>
+      <c r="G209" s="12"/>
+      <c r="H209" s="12"/>
+      <c r="I209" s="12"/>
+      <c r="J209" s="12"/>
+      <c r="K209" s="12"/>
+      <c r="L209" s="12"/>
+      <c r="M209" s="12"/>
+      <c r="N209" s="12"/>
+      <c r="O209" s="12"/>
+      <c r="P209" s="12"/>
+      <c r="Q209" s="12"/>
+      <c r="R209" s="12"/>
+      <c r="S209" s="12"/>
+      <c r="T209" s="12"/>
+      <c r="U209" s="12"/>
+      <c r="V209" s="12"/>
+      <c r="W209" s="12"/>
+      <c r="X209" s="12"/>
+      <c r="Y209" s="12"/>
+      <c r="Z209" s="12"/>
+      <c r="AA209" s="12"/>
+      <c r="AB209" s="12"/>
+      <c r="AC209" s="12"/>
+      <c r="AD209" s="12"/>
+      <c r="AE209" s="12"/>
+      <c r="AF209" s="12"/>
+      <c r="AG209" s="12"/>
+      <c r="AH209" s="12"/>
+      <c r="AI209" s="12"/>
+      <c r="AJ209" s="12"/>
+      <c r="AK209" s="12"/>
+    </row>
+    <row r="210" spans="1:37" s="13" customFormat="1">
+      <c r="A210" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B210" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C210" s="12"/>
+      <c r="D210" s="12"/>
+      <c r="E210" s="12"/>
+      <c r="F210" s="12"/>
+      <c r="G210" s="12"/>
+      <c r="H210" s="12"/>
+      <c r="I210" s="12"/>
+      <c r="J210" s="12"/>
+      <c r="K210" s="12"/>
+      <c r="L210" s="12"/>
+      <c r="M210" s="12"/>
+      <c r="N210" s="12"/>
+      <c r="O210" s="12"/>
+      <c r="P210" s="12"/>
+      <c r="Q210" s="12"/>
+      <c r="R210" s="12"/>
+      <c r="S210" s="12"/>
+      <c r="T210" s="12"/>
+      <c r="U210" s="12"/>
+      <c r="V210" s="12"/>
+      <c r="W210" s="12"/>
+      <c r="X210" s="12"/>
+      <c r="Y210" s="12"/>
+      <c r="Z210" s="12"/>
+      <c r="AA210" s="12"/>
+      <c r="AB210" s="12"/>
+      <c r="AC210" s="12"/>
+      <c r="AD210" s="12"/>
+      <c r="AE210" s="12"/>
+      <c r="AF210" s="12"/>
+      <c r="AG210" s="12"/>
+      <c r="AH210" s="12"/>
+      <c r="AI210" s="12"/>
+      <c r="AJ210" s="12"/>
+      <c r="AK210" s="12"/>
+    </row>
+    <row r="211" spans="1:37" s="13" customFormat="1">
+      <c r="A211" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B211" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C211" s="12"/>
+      <c r="D211" s="12"/>
+      <c r="E211" s="12"/>
+      <c r="F211" s="12"/>
+      <c r="G211" s="12"/>
+      <c r="H211" s="12"/>
+      <c r="I211" s="12"/>
+      <c r="J211" s="12"/>
+      <c r="K211" s="12"/>
+      <c r="L211" s="12"/>
+      <c r="M211" s="12"/>
+      <c r="N211" s="12"/>
+      <c r="O211" s="12"/>
+      <c r="P211" s="12"/>
+      <c r="Q211" s="12"/>
+      <c r="R211" s="12"/>
+      <c r="S211" s="12"/>
+      <c r="T211" s="12"/>
+      <c r="U211" s="12"/>
+      <c r="V211" s="12"/>
+      <c r="W211" s="12"/>
+      <c r="X211" s="12"/>
+      <c r="Y211" s="12"/>
+      <c r="Z211" s="12"/>
+      <c r="AA211" s="12"/>
+      <c r="AB211" s="12"/>
+      <c r="AC211" s="12"/>
+      <c r="AD211" s="12"/>
+      <c r="AE211" s="12"/>
+      <c r="AF211" s="12"/>
+      <c r="AG211" s="12"/>
+      <c r="AH211" s="12"/>
+      <c r="AI211" s="12"/>
+      <c r="AJ211" s="12"/>
+      <c r="AK211" s="12"/>
+    </row>
+    <row r="212" spans="1:37" s="13" customFormat="1">
+      <c r="A212" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B212" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C212" s="12"/>
+      <c r="D212" s="12"/>
+      <c r="E212" s="12"/>
+      <c r="F212" s="12"/>
+      <c r="G212" s="12"/>
+      <c r="H212" s="12"/>
+      <c r="I212" s="12"/>
+      <c r="J212" s="12"/>
+      <c r="K212" s="12"/>
+      <c r="L212" s="12"/>
+      <c r="M212" s="12"/>
+      <c r="N212" s="12"/>
+      <c r="O212" s="12"/>
+      <c r="P212" s="12"/>
+      <c r="Q212" s="12"/>
+      <c r="R212" s="12"/>
+      <c r="S212" s="12"/>
+      <c r="T212" s="12"/>
+      <c r="U212" s="12"/>
+      <c r="V212" s="12"/>
+      <c r="W212" s="12"/>
+      <c r="X212" s="12"/>
+      <c r="Y212" s="12"/>
+      <c r="Z212" s="12"/>
+      <c r="AA212" s="12"/>
+      <c r="AB212" s="12"/>
+      <c r="AC212" s="12"/>
+      <c r="AD212" s="12"/>
+      <c r="AE212" s="12"/>
+      <c r="AF212" s="12"/>
+      <c r="AG212" s="12"/>
+      <c r="AH212" s="12"/>
+      <c r="AI212" s="12"/>
+      <c r="AJ212" s="12"/>
+      <c r="AK212" s="12"/>
+    </row>
+    <row r="213" spans="1:37" s="13" customFormat="1">
+      <c r="A213" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B213" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="214" spans="1:37" s="13" customFormat="1">
+      <c r="A214" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B214" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="215" spans="1:37" s="13" customFormat="1">
+      <c r="A215" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B215" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="216" spans="1:37" s="13" customFormat="1">
+      <c r="A216" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B216" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="217" spans="1:37" s="13" customFormat="1">
+      <c r="A217" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B217" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="218" spans="1:37" s="13" customFormat="1">
+      <c r="A218" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B218" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="219" spans="1:37" s="13" customFormat="1">
+      <c r="A219" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B219" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="220" spans="1:37" s="1" customFormat="1">
+      <c r="A220" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S220" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:37" s="2" customFormat="1">
+      <c r="A221" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="S221" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:37" s="2" customFormat="1">
+      <c r="A222" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="S222" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:37" s="1" customFormat="1">
+      <c r="A223" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S223" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:37" s="1" customFormat="1">
+      <c r="A224" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S224" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:19" s="2" customFormat="1">
+      <c r="A225" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="S225" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6776,16 +8305,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6816,7 +8346,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>243</v>
       </c>
       <c r="B2" t="s">
         <v>126</v>
@@ -6825,57 +8355,54 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>109</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
         <v>126</v>
       </c>
-      <c r="D3" t="s">
-        <v>24</v>
+      <c r="D3" t="b">
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>126</v>
       </c>
-      <c r="C5" t="s">
-        <v>127</v>
-      </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>126</v>
@@ -6887,12 +8414,12 @@
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>187</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
         <v>126</v>
@@ -6904,12 +8431,12 @@
         <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
         <v>126</v>
@@ -6921,12 +8448,12 @@
         <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
         <v>126</v>
@@ -6938,12 +8465,12 @@
         <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>186</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="B10" t="s">
         <v>126</v>
@@ -6955,12 +8482,12 @@
         <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>126</v>
@@ -6972,12 +8499,12 @@
         <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>126</v>
@@ -6989,26 +8516,29 @@
         <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
         <v>126</v>
       </c>
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
       <c r="D13" t="s">
         <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>126</v>
@@ -7017,26 +8547,26 @@
         <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>176</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
         <v>126</v>
       </c>
-      <c r="C15" t="s">
-        <v>128</v>
-      </c>
       <c r="D15" t="s">
         <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
         <v>126</v>
@@ -7048,9 +8578,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
         <v>126</v>
@@ -7062,9 +8592,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
         <v>126</v>
@@ -7076,9 +8606,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
         <v>126</v>
@@ -7090,9 +8620,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B20" t="s">
         <v>126</v>
@@ -7100,31 +8630,153 @@
       <c r="C20" t="s">
         <v>128</v>
       </c>
-      <c r="D20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>152</v>
       </c>
       <c r="B21" t="s">
         <v>126</v>
       </c>
-      <c r="G21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B22" t="s">
         <v>126</v>
       </c>
       <c r="G22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" t="s">
         <v>208</v>
       </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D26" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7254,7 +8906,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
fix(emx): Make transcript,cdna and protein text datatype
</commit_message>
<xml_diff>
--- a/emx/vkgl-model.xlsx
+++ b/emx/vkgl-model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12980" yWindow="-16000" windowWidth="25600" windowHeight="14280" tabRatio="756" activeTab="4"/>
+    <workbookView xWindow="24220" yWindow="-18780" windowWidth="25600" windowHeight="15140" tabRatio="756"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -1489,9 +1489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK225"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U159" sqref="U159"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2139,7 +2139,7 @@
         <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
         <v>24</v>
@@ -2177,7 +2177,7 @@
         <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
@@ -2215,7 +2215,7 @@
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
@@ -3409,7 +3409,7 @@
         <v>43</v>
       </c>
       <c r="D49" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F49" t="s">
         <v>24</v>
@@ -3523,7 +3523,7 @@
         <v>45</v>
       </c>
       <c r="D52" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F52" t="s">
         <v>24</v>
@@ -3561,7 +3561,7 @@
         <v>47</v>
       </c>
       <c r="D53" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F53" t="s">
         <v>24</v>
@@ -6813,7 +6813,7 @@
         <v>43</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F152" s="8" t="s">
         <v>24</v>
@@ -6830,7 +6830,7 @@
         <v>47</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F153" s="8" t="s">
         <v>24</v>
@@ -6847,7 +6847,7 @@
         <v>45</v>
       </c>
       <c r="D154" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F154" s="8" t="s">
         <v>24</v>
@@ -8905,7 +8905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>

</xml_diff>